<commit_message>
Added COG outputs and functional group analysis
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Squirrel_MetaG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40EEFA8-18E5-442A-A5A5-37584F37C61F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50AFA1E-6333-4CE5-858F-ED9E45313B47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{6F41704D-6EA5-4DA9-864B-5ED36218732F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Season</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Hibernation</t>
+  </si>
+  <si>
+    <t>SubSeason</t>
   </si>
 </sst>
 </file>
@@ -397,23 +406,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9AEA658-E250-482E-A972-D8AEB4396335}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3715</v>
       </c>
@@ -423,8 +435,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3717</v>
       </c>
@@ -434,8 +449,11 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3723</v>
       </c>
@@ -445,8 +463,11 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3733</v>
       </c>
@@ -456,8 +477,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3734</v>
       </c>
@@ -467,8 +491,11 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3744</v>
       </c>
@@ -478,8 +505,11 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3772</v>
       </c>
@@ -489,8 +519,11 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3773</v>
       </c>
@@ -500,8 +533,11 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3775</v>
       </c>
@@ -510,6 +546,9 @@
       </c>
       <c r="C10" t="s">
         <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed SubSeason (Active/Hib) to Diet (Feeding/Fasting)
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Squirrel_MetaG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50AFA1E-6333-4CE5-858F-ED9E45313B47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADA96F9-4944-4A5D-8DEB-779B136B94A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" xr2:uid="{6F41704D-6EA5-4DA9-864B-5ED36218732F}"/>
   </bookViews>
@@ -48,13 +48,13 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Hibernation</t>
-  </si>
-  <si>
-    <t>SubSeason</t>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>Feeding</t>
+  </si>
+  <si>
+    <t>Fasting</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,7 +422,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -450,7 +450,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -464,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -478,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -492,7 +492,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -506,7 +506,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -520,7 +520,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -534,7 +534,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>